<commit_message>
new commit, all stuff.
</commit_message>
<xml_diff>
--- a/Python/final/grassDataWallsShort.xlsx
+++ b/Python/final/grassDataWallsShort.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morr0289\Documents\GitHub\RobotArm\Python\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FFE88C-59FE-4B35-B739-0A720D1FB08E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FFF33-56B8-4B5E-9C4A-A5056517DC45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21793" windowHeight="7700" xr2:uid="{D50A2E6F-7147-4860-A759-9944D9C5AA96}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>espeed</t>
   </si>
   <si>
-    <t>direction</t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>roll</t>
+  </si>
+  <si>
+    <t>dir</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:M251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -438,10 +438,10 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -453,16 +453,16 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">

</xml_diff>